<commit_message>
Se agrego tipo de cheque y formatos
</commit_message>
<xml_diff>
--- a/public/excel/file.xlsx
+++ b/public/excel/file.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="480" yWindow="108" windowWidth="4596" windowHeight="3144"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="INFO" sheetId="1" r:id="rId1"/>
+    <sheet name="TIPOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -48,9 +47,6 @@
     <t>F/909900</t>
   </si>
   <si>
-    <t>NOMINAL</t>
-  </si>
-  <si>
     <t>ANDRES ALVARADO</t>
   </si>
   <si>
@@ -58,13 +54,31 @@
   </si>
   <si>
     <t>OTRO</t>
+  </si>
+  <si>
+    <t>KENDRY FINOL</t>
+  </si>
+  <si>
+    <t>A LA ORDEN</t>
+  </si>
+  <si>
+    <t>AL PORTADOR</t>
+  </si>
+  <si>
+    <t>NOMINATIVO</t>
+  </si>
+  <si>
+    <t>OPCION</t>
+  </si>
+  <si>
+    <t>TIPO DE CHEQUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +86,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,11 +125,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -106,11 +162,47 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
@@ -123,17 +215,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5">
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
   </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" name="NOMBRE"/>
-    <tableColumn id="2" name="FECHA" dataDxfId="1"/>
-    <tableColumn id="3" name="MONTO" dataDxfId="0"/>
+    <tableColumn id="2" name="FECHA" dataDxfId="6"/>
+    <tableColumn id="3" name="MONTO" dataDxfId="5"/>
     <tableColumn id="4" name="DESCRIPCION"/>
-    <tableColumn id="5" name="TIPO"/>
+    <tableColumn id="5" name="TIPO" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A2:B6" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A2:B6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="OPCION" dataDxfId="4"/>
+    <tableColumn id="2" name="TIPO DE CHEQUE" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -424,17 +527,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -467,8 +572,8 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="E2" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -484,13 +589,13 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
+      <c r="E3" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4">
         <v>42829</v>
@@ -499,10 +604,27 @@
         <v>150000</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>31405</v>
+      </c>
+      <c r="C5" s="7">
+        <v>159678542</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
+      <c r="E5" s="13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -516,24 +638,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>